<commit_message>
Use new handle code
</commit_message>
<xml_diff>
--- a/xlloption.xlsx
+++ b/xlloption.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalx\source\repos\xlladdins\xlloption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C4F52-F31F-4EB3-AC5A-703580B9F85F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F83E474-A3E7-4A41-9913-0EEC2889585B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8055" yWindow="1785" windowWidth="20595" windowHeight="13215" activeTab="1" xr2:uid="{44AEB816-CB2A-4A0A-B718-E5B5191DFF2A}"/>
+    <workbookView xWindow="8145" yWindow="915" windowWidth="20595" windowHeight="13215" activeTab="1" xr2:uid="{44AEB816-CB2A-4A0A-B718-E5B5191DFF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Option" sheetId="2" r:id="rId1"/>
@@ -20,14 +20,14 @@
     <definedName name="delta">Check!$C$15:$G$15</definedName>
     <definedName name="dN">Check!$C$10:$K$10</definedName>
     <definedName name="dN_">Check!$C$11:$K$11</definedName>
-    <definedName name="eps">Check!$C$13</definedName>
+    <definedName name="eps">Check!$C$3</definedName>
     <definedName name="f" localSheetId="0">Option!$C$5</definedName>
     <definedName name="f">Check!$C$4:$K$4</definedName>
     <definedName name="gamma">Check!$C$16:$G$16</definedName>
     <definedName name="k" localSheetId="0">Option!$C$7</definedName>
     <definedName name="k">Check!$C$6:$K$6</definedName>
     <definedName name="m" localSheetId="0">Option!$C$4</definedName>
-    <definedName name="m">Check!#REF!</definedName>
+    <definedName name="m">Check!$C$18</definedName>
     <definedName name="N">Check!$C$8:$K$8</definedName>
     <definedName name="N_">Check!$C$9:$K$9</definedName>
     <definedName name="s" localSheetId="0">Option!$C$6</definedName>
@@ -141,7 +141,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,8 +170,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +191,13 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -240,13 +253,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -254,7 +283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -273,7 +301,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -282,16 +313,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="5" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="3" builtinId="21"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -606,9 +635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1DE0E9-42ED-434D-9763-27344F6A1B8E}">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -617,7 +644,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>20</v>
       </c>
     </row>
@@ -625,9 +652,9 @@
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <f>_xll.VARIATE.NORMAL()</f>
-        <v>1308484367552</v>
+        <v>2043202465984</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -651,30 +678,30 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -682,94 +709,94 @@
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <f>_xll.OPTION.CALL.VALUE(m, f, s, k)</f>
-        <v>7.9655674554058038</v>
-      </c>
-      <c r="D11" s="12">
+        <v>13.589108116054796</v>
+      </c>
+      <c r="D11" s="11">
         <f>_xll.OPTION.PUT.VALUE(m, f, s, k)</f>
-        <v>7.9655674554058038</v>
-      </c>
-      <c r="E11" s="12">
+        <v>3.5891081160547955</v>
+      </c>
+      <c r="E11" s="11">
         <f>_xll.OPTION.DIGITAL_CALL.VALUE(m, f, s, k)</f>
-        <v>0.46017216272297101</v>
-      </c>
-      <c r="F11" s="12">
+        <v>0.66523843579723096</v>
+      </c>
+      <c r="F11" s="11">
         <f>_xll.OPTION.DIGITAL_PUT.VALUE(m, f, s, k)</f>
-        <v>0.53982783727702899</v>
+        <v>0.33476156420276904</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <f>_xll.OPTION.CALL.DELTA(m, f, s, k)</f>
-        <v>0.53982783727702899</v>
-      </c>
-      <c r="D12" s="12">
+        <v>0.73460567337805582</v>
+      </c>
+      <c r="D12" s="11">
         <f>_xll.OPTION.PUT.DELTA(m, f, s, k)</f>
-        <v>-0.46017216272297101</v>
-      </c>
-      <c r="E12" s="12">
+        <v>-0.26539432662194418</v>
+      </c>
+      <c r="E12" s="11">
         <f>_xll.OPTION.DIGITAL_CALL.DELTA(m, f, s, k)</f>
-        <v>1.9847627373850589E-2</v>
-      </c>
-      <c r="F12" s="12">
+        <v>1.6389546714475921E-2</v>
+      </c>
+      <c r="F12" s="11">
         <f>_xll.OPTION.DIGITAL_PUT.DELTA(m, f, s, k)</f>
-        <v>-1.9847627373850589E-2</v>
+        <v>-1.6389546714475921E-2</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <f>_xll.OPTION.GAMMA(m, f, s, k)</f>
-        <v>1.9847627373850589E-2</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12">
+        <v>1.6389546714475921E-2</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11">
         <f>_xll.OPTION.DIGITAL_CALL.GAMMA(m, f, s, k)</f>
-        <v>9.9238136869252928E-4</v>
-      </c>
-      <c r="F13" s="12">
+        <v>9.1053037302644014E-4</v>
+      </c>
+      <c r="F13" s="11">
         <f>_xll.OPTION.DIGITAL_PUT.GAMMA(m, f, s, k)</f>
-        <v>-9.9238136869252928E-4</v>
+        <v>-9.1053037302644014E-4</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <f>_xll.OPTION.VEGA(m, f, s, k)</f>
-        <v>39.695254747701178</v>
-      </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12">
+        <v>32.779093428951846</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11">
         <f>_xll.OPTION.DIGITAL_CALL.VEGA(m, f, s, k)</f>
-        <v>-0.19847627373850585</v>
-      </c>
-      <c r="F14" s="12">
+        <v>-1.1414455708470743</v>
+      </c>
+      <c r="F14" s="11">
         <f>_xll.OPTION.DIGITAL_PUT.VEGA(m, f, s, k)</f>
-        <v>0.19847627373850585</v>
+        <v>1.1414455708470743</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f>(C11-D11)-(f-k)</f>
         <v>0</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <f>E11+F11-1</f>
         <v>0</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -786,7 +813,7 @@
   <dimension ref="B2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,20 +824,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="15" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1E-3</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
@@ -840,7 +873,7 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="13">
         <v>100</v>
       </c>
       <c r="D4">
@@ -880,7 +913,7 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="13">
         <v>0.2</v>
       </c>
       <c r="D5">
@@ -920,7 +953,7 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="13">
         <v>90</v>
       </c>
       <c r="D6">
@@ -960,189 +993,177 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f t="array" ref="C7:K7">(LN(k/f) + s*s/2)/s</f>
         <v>-0.42680257828913137</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>-0.42685257803913312</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>-0.42675257803912947</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>-0.42368166993943418</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>-0.4299498274262627</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>-0.42685257803913312</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>-0.42675257803912947</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>-0.42368166993943418</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>-0.4299498274262627</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="3"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f t="array" ref="C8:K8">_xlfn.NORM.S.DIST(x,TRUE)</f>
         <v>0.33476156420276892</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.33474335388067344</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.33477977509558732</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>0.33589899246019439</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>0.3336160692397333</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>0.33474335388067344</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>0.33477977509558732</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>0.33589899246019439</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>0.3336160692397333</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="3"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <f t="array" ref="C9:K9">_xlfn.NORM.S.DIST(x - s,TRUE)</f>
         <v>0.26539432662194407</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.26537793741400351</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>0.26541071650743053</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>0.26609000294045437</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0.2646909518045355</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>0.26537793741400351</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>0.26541071650743053</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>0.26609000294045437</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>0.2646909518045355</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="3"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <f t="array" ref="C10:K10">_xlfn.NORM.S.DIST(x,FALSE)</f>
         <v>0.3642121492105761</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.36420437654290005</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.3642199212113077</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0.36469583122619975</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0.36372144683295959</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0.36420437654290005</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>0.3642199212113077</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>0.36469583122619975</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>0.36372144683295959</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="3"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <f t="array" ref="C11:K11">_xlfn.NORM.S.DIST(x - s,FALSE)</f>
         <v>0.3277909342895185</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>0.32778066108199921</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.32780120710224797</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.32822624810357981</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0.32734930214966362</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>0.32778066108199921</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>0.32780120710224797</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>0.32822624810357981</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>0.32734930214966362</v>
       </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="20" t="s">
+      <c r="M11" s="3"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="19">
-        <v>1E-3</v>
-      </c>
-      <c r="D13" s="3">
-        <f>eps^2</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="L13" s="20" t="s">
+      <c r="L13" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1150,40 +1171,40 @@
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <f t="array" ref="C14:G14">k*N-f*N_</f>
         <v>3.5891081160547955</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>3.5888427299228418</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>3.5893735185763127</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>3.6219090273720589</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>3.5563510511224479</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f>H8</f>
         <v>0.33474335388067344</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <f t="shared" ref="I14:K14" si="3">I8</f>
         <v>0.33477977509558732</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <f t="shared" si="3"/>
         <v>0.33589899246019439</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <f t="shared" si="3"/>
         <v>0.3336160692397333</v>
       </c>
-      <c r="L14" s="4">
-        <f>C8</f>
+      <c r="L14" s="3">
+        <f t="array" ref="L14">N</f>
         <v>0.33476156420276892</v>
       </c>
     </row>
@@ -1191,37 +1212,37 @@
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <f>-N_</f>
         <v>-0.26539432662194407</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
       <c r="L15">
-        <f>-C10/(C4*C5)</f>
-        <v>-1.8210607460528806E-2</v>
+        <f t="array" ref="L15">-dN_/(f*s)</f>
+        <v>-1.6389546714475924E-2</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <f t="array" ref="C16">_xlfn.NORM.S.DIST(x-s,FALSE)/(f*s)</f>
         <v>1.6389546714475924E-2</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
       <c r="L16">
-        <f>-C10/(C4*C5)^2</f>
+        <f t="array" ref="L16">-dN/(f*s)^2</f>
         <v>-9.1053037302644025E-4</v>
       </c>
     </row>
@@ -1229,28 +1250,28 @@
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <f>f*_xlfn.NORM.S.DIST(x - s,FALSE)</f>
         <v>32.779093428951853</v>
       </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4">
-        <f>-C11*(C7- C5)/C5</f>
-        <v>1.027301013762367</v>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3">
+        <f t="array" ref="L17">-dN*(x - s)/s</f>
+        <v>1.1414455708470745</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="14">
         <f>_xll.VARIATE.NORMAL()</f>
-        <v>1308757923104</v>
-      </c>
-      <c r="K18" s="4"/>
+        <v>2043202466656</v>
+      </c>
+      <c r="K18" s="3"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
@@ -1260,35 +1281,35 @@
         <f>_xll.OPTION.IMPLIED(C18, C4, C14, C6)</f>
         <v>0.2000000000000198</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="10"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="4"/>
+      <c r="D21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="I21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1296,19 +1317,19 @@
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="4">
-        <f>_xll.OPTION.PUT.VALUE($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="F22" s="3">
+        <f t="array" ref="F22">_xll.OPTION.PUT.VALUE(m,f,s,k)</f>
         <v>3.5891081160547955</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="20">
         <f>C14-F22</f>
         <v>0</v>
       </c>
-      <c r="J22" s="4">
-        <f>_xll.OPTION.DIGITAL_PUT.VALUE($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="J22" s="3">
+        <f t="array" ref="J22">_xll.OPTION.DIGITAL_PUT.VALUE(m,f,s,k)</f>
         <v>0.33476156420276904</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="20">
         <f>J22-L14</f>
         <v>0</v>
       </c>
@@ -1317,19 +1338,19 @@
       <c r="B23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <f>(D14-E14)/(2*eps)</f>
         <v>-0.26539432673544638</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="19">
         <f>C15-D23</f>
         <v>1.1350231865492333E-10</v>
       </c>
-      <c r="F23" s="4">
-        <f>_xll.OPTION.PUT.DELTA($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="F23" s="3">
+        <f t="array" ref="F23">_xll.OPTION.PUT.DELTA(m,f,s,k)</f>
         <v>-0.26539432662194418</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="20">
         <f>C15-F23</f>
         <v>0</v>
       </c>
@@ -1337,15 +1358,15 @@
         <f>(H14-I14)/(2*eps)</f>
         <v>-1.8210607456936589E-2</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="21">
         <f>H23-L15</f>
-        <v>3.5922168017954448E-12</v>
-      </c>
-      <c r="J23" s="4">
-        <f>_xll.OPTION.DIGITAL_PUT.DELTA($C$18,$C$4,$C$5,$C$6)</f>
-        <v>-1.8210607460528803E-2</v>
-      </c>
-      <c r="K23">
+        <v>-1.8210607424606652E-3</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="array" ref="J23">_xll.OPTION.DIGITAL_PUT.DELTA(m,f,s,k)</f>
+        <v>-1.6389546714475921E-2</v>
+      </c>
+      <c r="K23" s="21">
         <f>J23-L15</f>
         <v>0</v>
       </c>
@@ -1354,19 +1375,19 @@
       <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <f>(D14-2*C14+E14)/(eps*eps)</f>
         <v>1.6389563484153769E-2</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="19">
         <f>C16-D24</f>
         <v>-1.6769677844280517E-8</v>
       </c>
-      <c r="F24" s="4">
-        <f>_xll.OPTION.GAMMA($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="F24" s="3">
+        <f t="array" ref="F24">_xll.OPTION.GAMMA(m,f,s,k)</f>
         <v>1.6389546714475921E-2</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="20">
         <f>C16-F24</f>
         <v>0</v>
       </c>
@@ -1374,15 +1395,15 @@
         <f>(H14-2*L14+I14)/(eps*eps)</f>
         <v>5.7072291337334491E-4</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="21">
         <f t="shared" ref="I24:I25" si="4">H24-L16</f>
         <v>1.481253286399785E-3</v>
       </c>
-      <c r="J24" s="4">
-        <f>_xll.OPTION.DIGITAL_PUT.GAMMA($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="J24" s="3">
+        <f t="array" ref="J24">_xll.OPTION.DIGITAL_PUT.GAMMA(m,f,s,k)</f>
         <v>-9.1053037302644014E-4</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="21">
         <f>J24-L16</f>
         <v>0</v>
       </c>
@@ -1391,19 +1412,19 @@
       <c r="B25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <f>(F14-G14)/(2*eps)</f>
         <v>32.778988124805508</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="19">
         <f>C17-D25</f>
         <v>1.0530414634501994E-4</v>
       </c>
-      <c r="F25" s="4">
-        <f>_xll.OPTION.VEGA($C$18,$C$4,$C$5,$C$6)</f>
+      <c r="F25" s="3">
+        <f t="array" ref="F25">_xll.OPTION.VEGA(m,f,s,k)</f>
         <v>32.779093428951846</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="20">
         <f>C17-F25</f>
         <v>0</v>
       </c>
@@ -1411,15 +1432,15 @@
         <f>(J14-K14)/(2*eps)</f>
         <v>1.141461610230543</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="21">
         <f t="shared" si="4"/>
-        <v>0.114160596468176</v>
-      </c>
-      <c r="J25" s="4">
-        <f>_xll.OPTION.DIGITAL_PUT.VEGA($C$18,$C$4,$C$5,$C$6)</f>
-        <v>1.0273010137623668</v>
-      </c>
-      <c r="K25">
+        <v>1.6039383468502422E-5</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="array" ref="J25">_xll.OPTION.DIGITAL_PUT.VEGA(m,f,s,k)</f>
+        <v>1.1414455708470743</v>
+      </c>
+      <c r="K25" s="21">
         <f>J25-L17</f>
         <v>0</v>
       </c>

</xml_diff>